<commit_message>
Add comments to recursion sheet
</commit_message>
<xml_diff>
--- a/en/05_programming_fundamentals/memory_example_4/example_memory.xlsx
+++ b/en/05_programming_fundamentals/memory_example_4/example_memory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\uniCourse_dataStructuresAndAlgorithms\en\05_programming_fundamentals\memory_example_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4444AD46-9A2B-411E-8D76-E8533C345028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0D00DB-FBAA-49D1-B55E-070FB956816A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{B0555C02-20C0-46F3-A1E0-B668F9422BC6}"/>
   </bookViews>
@@ -40,6 +40,30 @@
     <author>Anton Curmanschii</author>
   </authors>
   <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{8E439C57-A6C9-4EC2-9E47-AF2B0A06395F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anton Curmanschii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note: The return addresses have been ignored for simplicity, but they are pushed on the stack, always.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{A9FAE471-294B-4A73-9F2A-7250F107B101}">
       <text>
         <r>
@@ -60,7 +84,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-The local variables of a function are sometimes called its "Lexical scope"</t>
+The local variables of a function are sometimes called its "Lexical scope"
+The name that refers to the memory of all local veriables is "Stack frame".</t>
         </r>
       </text>
     </comment>
@@ -1459,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7FCB09-E7E7-49EE-960F-8DB6DA63E396}">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>